<commit_message>
Repositorys created, NationRegistrationNumber Validation, Constructor of models
</commit_message>
<xml_diff>
--- a/Documentatie/Prestaties Studenten Team.xlsx
+++ b/Documentatie/Prestaties Studenten Team.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Student</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Fixed connection met cloud MSSQL DB (hosting SmarterASP.Net)</t>
+  </si>
+  <si>
+    <t>Validation of NationRegistrationNumber en Constructor Models</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,6 +651,26 @@
         <v>14</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44623</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testdata Person aangevuld tot 100+
</commit_message>
<xml_diff>
--- a/Documentatie/Prestaties Studenten Team.xlsx
+++ b/Documentatie/Prestaties Studenten Team.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -132,13 +132,16 @@
     <t>Unit test document aangemaakt</t>
   </si>
   <si>
-    <t>Research + Team meeting</t>
-  </si>
-  <si>
-    <t>Resaerch + Team meeting</t>
-  </si>
-  <si>
     <t>security</t>
+  </si>
+  <si>
+    <t>Research security .Net + Team meeting</t>
+  </si>
+  <si>
+    <t>Code analyse + Team meeting</t>
+  </si>
+  <si>
+    <t>Test Data</t>
   </si>
 </sst>
 </file>
@@ -646,10 +649,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -811,7 +814,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,7 +831,41 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44683</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Database Diagram + prestaties
</commit_message>
<xml_diff>
--- a/Documentatie/Prestaties Studenten Team.xlsx
+++ b/Documentatie/Prestaties Studenten Team.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>Datum</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>CarView Update</t>
+  </si>
+  <si>
+    <t>Overlopen en verstaan code</t>
+  </si>
+  <si>
+    <t>prestantie</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Opmaak bijkomstige info</t>
   </si>
 </sst>
 </file>
@@ -703,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,6 +1000,74 @@
       </c>
       <c r="E16" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44729</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44730</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>